<commit_message>
Major changes for getting correlations
</commit_message>
<xml_diff>
--- a/CompareHumanData/ExperimentalResults_2.xlsx
+++ b/CompareHumanData/ExperimentalResults_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\JupyterN\VectorSymbolicArchitectures\CompareHumanData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58314FC0-8DB6-4FE1-A72D-98BBF7DFB74C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CD44752-CBCC-4B7A-A4A2-10C4A23F02C2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25135" windowHeight="9583" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1561,7 +1561,7 @@
   <dimension ref="A1:AI65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>

</xml_diff>